<commit_message>
added web logout unit
</commit_message>
<xml_diff>
--- a/AdvantageShopping/Default.xlsx
+++ b/AdvantageShopping/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="ChatBot" sheetId="6" r:id="rId6"/>
     <sheet name="Shipping_Login" sheetId="7" r:id="rId7"/>
     <sheet name="Mobile_Logout" sheetId="8" r:id="rId8"/>
+    <sheet name="Web_Logout" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -189,10 +190,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="283845"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -608,6 +609,25 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.95"/>
+  <cols>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>

</xml_diff>